<commit_message>
fix errors in dashboard
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Bikebites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF6F69E-912A-401F-BF3F-D858CCB81B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C916389-6C73-4BA3-B262-0B9B489991BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -8179,15 +8179,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>68580</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8303,8 +8303,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Martial status">
@@ -8327,7 +8327,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8381,8 +8381,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>15241</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="6" name="Occupation">
@@ -8405,7 +8405,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8459,8 +8459,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="7" name="Region">
@@ -8483,7 +8483,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -24683,476 +24683,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FC10E613-8E9B-4CF2-ADD1-B38AC0707168}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="A4:D8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="1"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="13"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Income" fld="3" subtotal="average" baseField="2" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="6" format="11" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="6" format="12" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3B5DA4A0-29F9-4761-A3D2-1DF68B9FF0B1}" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A68:D122" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="1"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="54">
-        <item x="37"/>
-        <item x="22"/>
-        <item x="40"/>
-        <item x="26"/>
-        <item x="19"/>
-        <item x="25"/>
-        <item x="23"/>
-        <item x="21"/>
-        <item x="6"/>
-        <item x="17"/>
-        <item x="11"/>
-        <item x="4"/>
-        <item x="34"/>
-        <item x="13"/>
-        <item x="32"/>
-        <item x="8"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item x="12"/>
-        <item x="30"/>
-        <item x="15"/>
-        <item x="28"/>
-        <item x="38"/>
-        <item x="5"/>
-        <item x="36"/>
-        <item x="31"/>
-        <item x="39"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="42"/>
-        <item x="7"/>
-        <item x="14"/>
-        <item x="2"/>
-        <item x="33"/>
-        <item x="24"/>
-        <item x="18"/>
-        <item x="46"/>
-        <item x="27"/>
-        <item x="29"/>
-        <item x="41"/>
-        <item x="35"/>
-        <item x="45"/>
-        <item x="43"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="44"/>
-        <item x="48"/>
-        <item x="47"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="11"/>
-  </rowFields>
-  <rowItems count="53">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="13"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="13" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7272E39B-71EC-4692-9297-F5EFB3856DC9}" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7272E39B-71EC-4692-9297-F5EFB3856DC9}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A50:D55" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -25607,8 +25138,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24E2D324-2E39-4307-ABDA-325368E292E9}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24E2D324-2E39-4307-ABDA-325368E292E9}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A28:D35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -25742,6 +25273,475 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="2" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FC10E613-8E9B-4CF2-ADD1-B38AC0707168}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="A4:D8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="13"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Income" fld="3" subtotal="average" baseField="2" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3B5DA4A0-29F9-4761-A3D2-1DF68B9FF0B1}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A68:D122" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="54">
+        <item x="37"/>
+        <item x="22"/>
+        <item x="40"/>
+        <item x="26"/>
+        <item x="19"/>
+        <item x="25"/>
+        <item x="23"/>
+        <item x="21"/>
+        <item x="6"/>
+        <item x="17"/>
+        <item x="11"/>
+        <item x="4"/>
+        <item x="34"/>
+        <item x="13"/>
+        <item x="32"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item x="12"/>
+        <item x="30"/>
+        <item x="15"/>
+        <item x="28"/>
+        <item x="38"/>
+        <item x="5"/>
+        <item x="36"/>
+        <item x="31"/>
+        <item x="39"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="42"/>
+        <item x="7"/>
+        <item x="14"/>
+        <item x="2"/>
+        <item x="33"/>
+        <item x="24"/>
+        <item x="18"/>
+        <item x="46"/>
+        <item x="27"/>
+        <item x="29"/>
+        <item x="41"/>
+        <item x="35"/>
+        <item x="45"/>
+        <item x="43"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="44"/>
+        <item x="48"/>
+        <item x="47"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="53">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="13"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="13" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -26157,10 +26157,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
   <dimension ref="A1:N1001"/>
   <sheetViews>
     <sheetView topLeftCell="A722" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M735" sqref="M735"/>
+      <selection activeCell="H741" sqref="H741"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -71235,9 +71238,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D209F8-A052-4243-9AD6-0B61C393E36A}">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
   <dimension ref="A4:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
@@ -72248,15 +72254,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A596F25-F4A0-4795-85F1-37084C34CD3E}">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>